<commit_message>
Example R file for Uganda changed into txt file
</commit_message>
<xml_diff>
--- a/Scripts/August scripts/Definition of FNS indicators 2008-2012.xlsx
+++ b/Scripts/August scripts/Definition of FNS indicators 2008-2012.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="11475" windowHeight="9525" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="11475" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="3" r:id="rId1"/>
@@ -677,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,7 +759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -2779,7 +2779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>

</xml_diff>